<commit_message>
Updated optimization to dosomething and gave variables that sometimes were missing a value a defualt
</commit_message>
<xml_diff>
--- a/Zeus OS Workspace 2018 2.4/Zeus/data/TOP/Results/TOP7.4.t_long_HighestDemandInReachableArea.xlsx
+++ b/Zeus OS Workspace 2018 2.4/Zeus/data/TOP/Results/TOP7.4.t_long_HighestDemandInReachableArea.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Depot #0</t>
   </si>
@@ -29,7 +29,7 @@
     <t>Depot Total Distance: 26.565353393554688</t>
   </si>
   <si>
-    <t>Depot Total Trucks: 4</t>
+    <t>Depot Total Trucks: 3</t>
   </si>
   <si>
     <t>Truck #0</t>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>Truck Total Distance: 0.0</t>
-  </si>
-  <si>
-    <t>Truck #3</t>
   </si>
   <si>
     <t>Depot #1</t>
@@ -317,50 +314,19 @@
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F12" t="s">
         <v>28</v>
-      </c>
-      <c r="F14" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>